<commit_message>
corrected error in Matt Kern's submission
</commit_message>
<xml_diff>
--- a/data-raw/submissions/mkern-template.xlsx
+++ b/data-raw/submissions/mkern-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tylerbradley/Documents/thrones-pool/data-raw/submissions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F905E85-FAD4-BC4F-AEFA-73D789DBB8F2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E081F954-6A7E-9B46-AB0C-FADEC4510891}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -200,49 +200,6 @@
   </si>
   <si>
     <t>Will we see an undead Ned Stark? (2) … yes or no answer</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Over / under how many Stark children survive: +1.5 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="9"/>
-        <rFont val="Helvetica Neue"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>?</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Helvetica Neue"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> (2)Over / under how many Stark children survive: +1.5 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="9"/>
-        <rFont val="Helvetica Neue"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>?</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Helvetica Neue"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> (2)</t>
-    </r>
   </si>
   <si>
     <r>
@@ -270,6 +227,30 @@
   </si>
   <si>
     <t>Who wins the Game of Thrones??? (5) **If only one person guesses correctly they win 20% of pool and a prize**</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Over / under how many Stark children survive: +1.5 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="9"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> (2)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -487,26 +468,26 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -913,8 +894,8 @@
   </sheetPr>
   <dimension ref="A1:IT43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" outlineLevelCol="1" x14ac:dyDescent="0.15"/>
@@ -927,13 +908,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="27.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
     </row>
     <row r="2" spans="1:8" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="3"/>
@@ -948,12 +929,12 @@
     </row>
     <row r="3" spans="1:8" ht="24.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="3"/>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
     </row>
     <row r="4" spans="1:8" ht="21.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="3"/>
@@ -1359,27 +1340,27 @@
     </row>
     <row r="25" spans="1:8" ht="24.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="3"/>
-      <c r="B25" s="22" t="s">
+      <c r="B25" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="C25" s="22"/>
-      <c r="D25" s="22"/>
-      <c r="E25" s="23" t="s">
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="F25" s="23"/>
-      <c r="G25" s="23"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="21"/>
       <c r="H25" s="13" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="20.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="3"/>
-      <c r="B26" s="17" t="s">
+      <c r="B26" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="C26" s="17"/>
-      <c r="D26" s="17"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="22"/>
       <c r="E26" s="15" t="s">
         <v>17</v>
       </c>
@@ -1389,11 +1370,11 @@
     </row>
     <row r="27" spans="1:8" ht="20.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="3"/>
-      <c r="B27" s="19" t="s">
+      <c r="B27" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="C27" s="19"/>
-      <c r="D27" s="19"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
       <c r="E27" s="15" t="s">
         <v>39</v>
       </c>
@@ -1403,11 +1384,11 @@
     </row>
     <row r="28" spans="1:8" ht="20.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="3"/>
-      <c r="B28" s="17" t="s">
+      <c r="B28" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="C28" s="17"/>
-      <c r="D28" s="17"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
       <c r="E28" s="16" t="s">
         <v>8</v>
       </c>
@@ -1417,11 +1398,11 @@
     </row>
     <row r="29" spans="1:8" ht="32" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="3"/>
-      <c r="B29" s="18" t="s">
+      <c r="B29" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
+      <c r="C29" s="23"/>
+      <c r="D29" s="23"/>
       <c r="E29" s="15" t="s">
         <v>51</v>
       </c>
@@ -1431,11 +1412,11 @@
     </row>
     <row r="30" spans="1:8" ht="31" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="3"/>
-      <c r="B30" s="18" t="s">
+      <c r="B30" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
+      <c r="C30" s="23"/>
+      <c r="D30" s="23"/>
       <c r="E30" s="15" t="s">
         <v>23</v>
       </c>
@@ -1445,11 +1426,11 @@
     </row>
     <row r="31" spans="1:8" ht="23" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="3"/>
-      <c r="B31" s="19" t="s">
+      <c r="B31" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="19"/>
-      <c r="D31" s="19"/>
+      <c r="C31" s="17"/>
+      <c r="D31" s="17"/>
       <c r="E31" s="16" t="s">
         <v>13</v>
       </c>
@@ -1459,11 +1440,11 @@
     </row>
     <row r="32" spans="1:8" ht="23" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="3"/>
-      <c r="B32" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
+      <c r="B32" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="C32" s="23"/>
+      <c r="D32" s="23"/>
       <c r="E32" s="16" t="s">
         <v>16</v>
       </c>
@@ -1473,11 +1454,11 @@
     </row>
     <row r="33" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="3"/>
-      <c r="B33" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
+      <c r="B33" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="C33" s="23"/>
+      <c r="D33" s="23"/>
       <c r="E33" s="16" t="s">
         <v>16</v>
       </c>
@@ -1487,11 +1468,11 @@
     </row>
     <row r="34" spans="1:8" ht="32.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="3"/>
-      <c r="B34" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="C34" s="17"/>
-      <c r="D34" s="17"/>
+      <c r="B34" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="C34" s="22"/>
+      <c r="D34" s="22"/>
       <c r="E34" s="15" t="s">
         <v>44</v>
       </c>
@@ -1547,12 +1528,6 @@
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="13">
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="E25:G25"/>
-    <mergeCell ref="B26:D26"/>
     <mergeCell ref="B34:D34"/>
     <mergeCell ref="B28:D28"/>
     <mergeCell ref="B29:D29"/>
@@ -1560,6 +1535,12 @@
     <mergeCell ref="B31:D31"/>
     <mergeCell ref="B32:D32"/>
     <mergeCell ref="B33:D33"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="E25:G25"/>
+    <mergeCell ref="B26:D26"/>
   </mergeCells>
   <dataValidations count="5">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C24 E5:E24" xr:uid="{00000000-0002-0000-0000-000000000000}">

</xml_diff>